<commit_message>
Port over some more of the examples.
</commit_message>
<xml_diff>
--- a/ObjectCacheDemo/ObjectCache.xlsx
+++ b/ObjectCacheDemo/ObjectCache.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\WorkSpace\xlw-Examples\ObjectCacheDemo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{08A7FB52-69A9-4788-8327-C9E7F1077366}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45383158-D0FA-41C6-A40C-4AFE3D69BAC9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="165" windowWidth="28800" windowHeight="15090"/>
+    <workbookView xWindow="195" yWindow="0" windowWidth="28800" windowHeight="15090" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,12 +22,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Narinder Claire</author>
   </authors>
   <commentList>
-    <comment ref="C9" authorId="0" shapeId="0">
+    <comment ref="C9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -51,7 +51,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D18" authorId="0" shapeId="0">
+    <comment ref="D18" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -76,7 +76,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H18" authorId="0" shapeId="0">
+    <comment ref="H18" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -105,7 +105,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
   <si>
     <t>a</t>
   </si>
@@ -145,13 +145,28 @@
   <si>
     <t>=Discount(G16,$M$16)</t>
   </si>
+  <si>
+    <t>Hello</t>
+  </si>
+  <si>
+    <t xml:space="preserve">How </t>
+  </si>
+  <si>
+    <t xml:space="preserve">are </t>
+  </si>
+  <si>
+    <t xml:space="preserve">you </t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -505,13 +520,13 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="10" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="10" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="10" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="10" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -857,11 +872,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C5:O41"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="C5:R41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AB12" sqref="AB12"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="R20" sqref="R20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1024,18 +1039,22 @@
       </c>
       <c r="M16" s="34">
         <f ca="1">TODAY()+32</f>
-        <v>44084</v>
-      </c>
-    </row>
-    <row r="17" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>44087</v>
+      </c>
+    </row>
+    <row r="17" spans="3:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C17" s="20" t="s">
         <v>4</v>
       </c>
       <c r="G17" s="33" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="18" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J17" t="str">
+        <f t="array" ref="J17">_xll.SendRange(O19:P20)</f>
+        <v>non error cell asked to be an error</v>
+      </c>
+    </row>
+    <row r="18" spans="3:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C18" s="21">
         <v>40113</v>
       </c>
@@ -1055,7 +1074,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C19" s="23">
         <v>40144</v>
       </c>
@@ -1071,15 +1090,15 @@
       <c r="L19" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="M19" s="37">
+      <c r="M19" s="37" t="e">
         <f ca="1">_xll.Discount(C16,$M$16)</f>
-        <v>0.92605475278334093</v>
+        <v>#NAME?</v>
       </c>
       <c r="O19" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="3:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C20" s="23">
         <v>40174</v>
       </c>
@@ -1095,15 +1114,15 @@
       <c r="L20" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="M20" s="39">
+      <c r="M20" s="39" t="e">
         <f ca="1">_xll.Discount(G16,$M$16)</f>
-        <v>0.98076278549167062</v>
+        <v>#NAME?</v>
       </c>
       <c r="O20" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C21" s="23">
         <v>40205</v>
       </c>
@@ -1117,7 +1136,7 @@
         <v>0.9972093804899117</v>
       </c>
     </row>
-    <row r="22" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C22" s="23">
         <v>40236</v>
       </c>
@@ -1131,7 +1150,7 @@
         <v>0.998</v>
       </c>
     </row>
-    <row r="23" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C23" s="23">
         <v>40264</v>
       </c>
@@ -1145,7 +1164,7 @@
         <v>0.99559875508719664</v>
       </c>
     </row>
-    <row r="24" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C24" s="23">
         <v>40295</v>
       </c>
@@ -1159,7 +1178,7 @@
         <v>0.9947807909362486</v>
       </c>
     </row>
-    <row r="25" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C25" s="23">
         <v>40325</v>
       </c>
@@ -1172,8 +1191,26 @@
       <c r="H25" s="30">
         <v>0.99393626730474738</v>
       </c>
-    </row>
-    <row r="26" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="M25" t="s">
+        <v>13</v>
+      </c>
+      <c r="N25" t="s">
+        <v>14</v>
+      </c>
+      <c r="O25" t="s">
+        <v>15</v>
+      </c>
+      <c r="P25" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>17</v>
+      </c>
+      <c r="R25" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="26" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C26" s="23">
         <v>40356</v>
       </c>
@@ -1186,8 +1223,32 @@
       <c r="H26" s="30">
         <v>0.99311966902072157</v>
       </c>
-    </row>
-    <row r="27" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="M26">
+        <f ca="1">RAND()</f>
+        <v>0.20243851269246693</v>
+      </c>
+      <c r="N26">
+        <f t="shared" ref="N26:R36" ca="1" si="0">RAND()</f>
+        <v>0.63159573058824259</v>
+      </c>
+      <c r="O26">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.40054784297223867</v>
+      </c>
+      <c r="P26">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.80889176174063848</v>
+      </c>
+      <c r="Q26">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.675153812255057</v>
+      </c>
+      <c r="R26">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.10896884009594232</v>
+      </c>
+    </row>
+    <row r="27" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C27" s="23">
         <v>40386</v>
       </c>
@@ -1200,8 +1261,32 @@
       <c r="H27" s="30">
         <v>0.99227655560614969</v>
       </c>
-    </row>
-    <row r="28" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="M27">
+        <f t="shared" ref="M27:M36" ca="1" si="1">RAND()</f>
+        <v>0.50418361483058993</v>
+      </c>
+      <c r="N27">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.14281843208150447</v>
+      </c>
+      <c r="O27">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.18549583208673326</v>
+      </c>
+      <c r="P27">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.34160186375671586</v>
+      </c>
+      <c r="Q27">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.98535318150358608</v>
+      </c>
+      <c r="R27">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.41357524639034859</v>
+      </c>
+    </row>
+    <row r="28" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C28" s="23">
         <v>40417</v>
       </c>
@@ -1214,8 +1299,32 @@
       <c r="H28" s="30">
         <v>0.99143415795650736</v>
       </c>
-    </row>
-    <row r="29" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="M28">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.34048369675403189</v>
+      </c>
+      <c r="N28">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.90152112596414935</v>
+      </c>
+      <c r="O28">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.96787323006910952</v>
+      </c>
+      <c r="P28">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.48348595114454018</v>
+      </c>
+      <c r="Q28">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.99952371170945831</v>
+      </c>
+      <c r="R28">
+        <f t="shared" ca="1" si="0"/>
+        <v>6.4229417555727086E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C29" s="23">
         <v>40448</v>
       </c>
@@ -1228,8 +1337,32 @@
       <c r="H29" s="30">
         <v>0.9906196153557959</v>
       </c>
-    </row>
-    <row r="30" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="M29">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.34029467037704608</v>
+      </c>
+      <c r="N29">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.27225625926690067</v>
+      </c>
+      <c r="O29">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.66223565535264306</v>
+      </c>
+      <c r="P29">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.76367952607748313</v>
+      </c>
+      <c r="Q29">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.33750071767993683</v>
+      </c>
+      <c r="R29">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.4276610832467781</v>
+      </c>
+    </row>
+    <row r="30" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C30" s="23">
         <v>40478</v>
       </c>
@@ -1242,8 +1375,32 @@
       <c r="H30" s="30">
         <v>0.98977862437303954</v>
       </c>
-    </row>
-    <row r="31" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="M30">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.14391269135604723</v>
+      </c>
+      <c r="N30">
+        <f t="shared" ca="1" si="0"/>
+        <v>1.01747364199537E-2</v>
+      </c>
+      <c r="O30">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.25014064163609995</v>
+      </c>
+      <c r="P30">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.81282724082785063</v>
+      </c>
+      <c r="Q30">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.63641019611905025</v>
+      </c>
+      <c r="R30">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.58786100968202581</v>
+      </c>
+    </row>
+    <row r="31" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C31" s="23">
         <v>40509</v>
       </c>
@@ -1256,8 +1413,32 @@
       <c r="H31" s="30">
         <v>0.9889654419258187</v>
       </c>
-    </row>
-    <row r="32" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="M31">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.21397682198006629</v>
+      </c>
+      <c r="N31">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.71957053961476869</v>
+      </c>
+      <c r="O31">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.63075181121786927</v>
+      </c>
+      <c r="P31">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.62195669814201016</v>
+      </c>
+      <c r="Q31">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.43267485702136887</v>
+      </c>
+      <c r="R31">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.36262613156525425</v>
+      </c>
+    </row>
+    <row r="32" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C32" s="23">
         <v>40539</v>
       </c>
@@ -1270,8 +1451,32 @@
       <c r="H32" s="30">
         <v>0.98812585526104368</v>
       </c>
-    </row>
-    <row r="33" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="M32">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.86768655446286347</v>
+      </c>
+      <c r="N32">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.49635695721077067</v>
+      </c>
+      <c r="O32">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.11418226876730175</v>
+      </c>
+      <c r="P32">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.41752610065103324</v>
+      </c>
+      <c r="Q32">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.56588084931123706</v>
+      </c>
+      <c r="R32">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.62383151461472108</v>
+      </c>
+    </row>
+    <row r="33" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C33" s="23">
         <v>40570</v>
       </c>
@@ -1284,8 +1489,32 @@
       <c r="H33" s="30">
         <v>0.98728698136714788</v>
       </c>
-    </row>
-    <row r="34" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="M33">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.27835990924097609</v>
+      </c>
+      <c r="N33">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.27743783176631953</v>
+      </c>
+      <c r="O33">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.63803047415808212</v>
+      </c>
+      <c r="P33">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.21045891908415892</v>
+      </c>
+      <c r="Q33">
+        <f t="shared" ca="1" si="0"/>
+        <v>8.0867549996369248E-2</v>
+      </c>
+      <c r="R33">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.98776013655859585</v>
+      </c>
+    </row>
+    <row r="34" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C34" s="23">
         <v>40601</v>
       </c>
@@ -1298,8 +1527,32 @@
       <c r="H34" s="30">
         <v>0.98652990095626059</v>
       </c>
-    </row>
-    <row r="35" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="M34">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.14970725650510397</v>
+      </c>
+      <c r="N34">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.33381577602804335</v>
+      </c>
+      <c r="O34">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.63271520243621338</v>
+      </c>
+      <c r="P34">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.67591760875754048</v>
+      </c>
+      <c r="Q34">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.78108665414413803</v>
+      </c>
+      <c r="R34">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.59405925741323862</v>
+      </c>
+    </row>
+    <row r="35" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C35" s="23">
         <v>40629</v>
       </c>
@@ -1312,8 +1565,32 @@
       <c r="H35" s="30">
         <v>0.98569238195495767</v>
       </c>
-    </row>
-    <row r="36" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="M35">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.15124840950111196</v>
+      </c>
+      <c r="N35">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.72452435537898263</v>
+      </c>
+      <c r="O35">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.41857740035035529</v>
+      </c>
+      <c r="P35">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.15968794456028035</v>
+      </c>
+      <c r="Q35">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.99624434107017301</v>
+      </c>
+      <c r="R35">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.94946732515901799</v>
+      </c>
+    </row>
+    <row r="36" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C36" s="23">
         <v>40660</v>
       </c>
@@ -1326,8 +1603,32 @@
       <c r="H36" s="30">
         <v>0.98488255668329883</v>
       </c>
-    </row>
-    <row r="37" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="M36">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.10586684864664964</v>
+      </c>
+      <c r="N36">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.42579602795496285</v>
+      </c>
+      <c r="O36">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.77833743192100913</v>
+      </c>
+      <c r="P36">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.16530734572501093</v>
+      </c>
+      <c r="Q36">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.31144038830280152</v>
+      </c>
+      <c r="R36">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.58376198034904703</v>
+      </c>
+    </row>
+    <row r="37" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C37" s="23">
         <v>40690</v>
       </c>
@@ -1341,7 +1642,7 @@
         <v>0.98404643620233379</v>
       </c>
     </row>
-    <row r="38" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C38" s="23">
         <v>40721</v>
       </c>
@@ -1355,7 +1656,7 @@
         <v>0.98323796320699419</v>
       </c>
     </row>
-    <row r="39" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C39" s="23">
         <v>40751</v>
       </c>
@@ -1369,7 +1670,7 @@
         <v>0.98240323891106562</v>
       </c>
     </row>
-    <row r="40" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C40" s="23">
         <v>40782</v>
       </c>
@@ -1383,7 +1684,7 @@
         <v>0.98156922325808649</v>
       </c>
     </row>
-    <row r="41" spans="3:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="3:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C41" s="25">
         <v>40813</v>
       </c>
@@ -1404,7 +1705,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1416,7 +1717,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>